<commit_message>
finalna wersja panelu Admina
</commit_message>
<xml_diff>
--- a/drugs.xlsx
+++ b/drugs.xlsx
@@ -424,56 +424,56 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ID,DRUG,ON_RECEPT,NO_PACKAGES_AVAILABLE,DATE</t>
+          <t>ID,DRUG,ON_RECEPT,NO_PACKAGES_AVAILABLE,DATE,RECEPT_ID</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1,POLOPIRYNA,NO,1200,2024-03-25 00:00:00</t>
+          <t>1,POLOPIRYNA,NO,1200,2024-03-25 00:00:00,nan</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3,AMOTAX,YES,336,2015-02-14 00:00:00</t>
+          <t>3,AMOTAX,YES,336,2015-02-14 00:00:00,nan</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5,GSGDF,YES,455,2025-05-24 19:55:06</t>
+          <t>5,GSGDF,YES,455,2025-05-24 19:55:06,nan</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>6,JHV,YES,4445,2025-05-25 09:19:09</t>
+          <t>6,JHV,YES,4445,2025-05-25 09:19:09,nan</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>7,RREWRW,NO,4432,2025-05-25 09:19:19</t>
+          <t>7,RREWRW,NO,4432,2025-05-25 09:19:19,nan</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>8,JGHJGH,YES,766,2025-05-25 09:19:25</t>
+          <t>10,EWQ,YES,232,2025-05-26 21:05:04,nan</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>9,SDA,YES,23,2025-05-26 18:01:41</t>
+          <t>12,SDSAD,YES,2311,2025-05-27 15:51:10,2344.0</t>
         </is>
       </c>
     </row>

</xml_diff>